<commit_message>
Update of cases' time series
</commit_message>
<xml_diff>
--- a/data-raw/EpiDataFrance.xlsx
+++ b/data-raw/EpiDataFrance.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6755" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6755" uniqueCount="193">
   <si>
     <t>80P</t>
   </si>
@@ -669,6 +669,18 @@
   <si>
     <t>Metropole</t>
   </si>
+  <si>
+    <t>Grand-Est</t>
+  </si>
+  <si>
+    <t>Auvergne-Rhone-Alpes</t>
+  </si>
+  <si>
+    <t>Bourgogne-Franche-Comte</t>
+  </si>
+  <si>
+    <t>PACA</t>
+  </si>
 </sst>
 </file>
 
@@ -1197,8 +1209,8 @@
   <dimension ref="A1:BM54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N54" sqref="N54"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1218,7 @@
     <col min="1" max="1" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="155.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:65" ht="151.5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>67</v>
       </c>
@@ -1214,10 +1226,10 @@
         <v>46</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>52</v>
+        <v>190</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>53</v>
+        <v>191</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>54</v>
@@ -1229,7 +1241,7 @@
         <v>56</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>57</v>
+        <v>189</v>
       </c>
       <c r="I1" s="20" t="s">
         <v>58</v>
@@ -1250,7 +1262,7 @@
         <v>63</v>
       </c>
       <c r="O1" s="20" t="s">
-        <v>64</v>
+        <v>192</v>
       </c>
       <c r="P1" s="20" t="s">
         <v>188</v>

</xml_diff>